<commit_message>
feat:done report pandu ptm hipertensi and diabetes
</commit_message>
<xml_diff>
--- a/public/assets/report/report-uspro.xlsx
+++ b/public/assets/report/report-uspro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laravel\sistem-pelaporan-terpadu-puskesmas\public\assets\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02647443-D930-4416-9B38-9E805A96CF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDCA236-6E26-414F-960B-32540AF061C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>PEMERINTAH KOTA MAKASSAR</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">LAPORAN KUNJUNGAN USIA PRODUKTIF (USPRO) 15 TAHUN S/D 59 TAHUN </t>
-  </si>
-  <si>
-    <t>BULAN MEI TAHUN 2025</t>
   </si>
   <si>
     <t>NO</t>
@@ -591,7 +588,7 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18:H19"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -748,9 +745,7 @@
       <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
@@ -767,34 +762,34 @@
     </row>
     <row r="11" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="I11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>